<commit_message>
Updated console log, fetch URLs, and CORS Setup
</commit_message>
<xml_diff>
--- a/server/dispatched_items_log.xlsx
+++ b/server/dispatched_items_log.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -710,9 +710,23 @@
         <v>13/6/2025, 10:29:48 pm</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>x1</v>
+      </c>
+      <c r="B23" t="str">
+        <v>Screwdriver</v>
+      </c>
+      <c r="C23" t="str">
+        <v>2025-06-14T03:22:22.333Z</v>
+      </c>
+      <c r="D23" t="str">
+        <v>14/6/2025, 8:52:22 am</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>